<commit_message>
modify EM algorithm in hlm, change to pure EM.
</commit_message>
<xml_diff>
--- a/data/hlm/train_erosion_data.xlsx
+++ b/data/hlm/train_erosion_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\PyProjects\simpleLearning\data\hlm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C91BE253-C567-4C4E-9F1C-609B22F976CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFCFE774-4B8A-4B06-8D62-3FC2D3148C74}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="13068" windowHeight="11340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7536" yWindow="420" windowWidth="13068" windowHeight="11340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="erosion" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="12">
   <si>
     <t>站点</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -398,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -477,6 +477,230 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>2.7890000000000001</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2.5139999999999998</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>2.298</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>2.1030000000000002</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>1.9870000000000001</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>1.766</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>1.625</v>
+      </c>
+      <c r="C12">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>1.4890000000000001</v>
+      </c>
+      <c r="C13">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>1.379</v>
+      </c>
+      <c r="C14">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>1.32</v>
+      </c>
+      <c r="C15">
+        <v>14</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>1.256</v>
+      </c>
+      <c r="C16">
+        <v>15</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>1.2010000000000001</v>
+      </c>
+      <c r="C17">
+        <v>16</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>1.155</v>
+      </c>
+      <c r="C18">
+        <v>17</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>1.1060000000000001</v>
+      </c>
+      <c r="C19">
+        <v>18</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>0.97899999999999998</v>
+      </c>
+      <c r="C20">
+        <v>19</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>0.89700000000000002</v>
+      </c>
+      <c r="C21">
+        <v>20</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -488,7 +712,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00DCABB9-246D-4449-B498-0CE3C5AF61CF}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:J2"/>
     </sheetView>
   </sheetViews>

</xml_diff>